<commit_message>
both files are modified
</commit_message>
<xml_diff>
--- a/a.xlsx
+++ b/a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SampleProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AACA9D-C0ED-46EF-A086-B655A9E07C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294133F7-68BA-46E4-A7B5-90E588E5FC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -337,10 +337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -362,6 +362,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>